<commit_message>
Testrail testdata demo class
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/FrameworkTest.xlsx
+++ b/src/test/resources/TestData/FrameworkTest.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1172" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1194" uniqueCount="416">
   <si>
     <t xml:space="preserve">TestName</t>
   </si>
@@ -1222,7 +1222,115 @@
     <t xml:space="preserve">searchInvalidCategory_POST_JSONTest</t>
   </si>
   <si>
+    <t xml:space="preserve">sending</t>
+  </si>
+  <si>
+    <t xml:space="preserve">orderNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tcIDs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dataProviderKey</t>
+  </si>
+  <si>
     <t xml:space="preserve">methodNameDemo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C222760,C222393,C222394,C222938</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Collection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C222391,C222393,C222394,C222395</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delivery</t>
+  </si>
+  <si>
+    <t xml:space="preserve">restaurant</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="13"/>
+        <color rgb="FF797979"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">C222392</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <color rgb="FF797979"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="13"/>
+        <color rgb="FF797979"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">C222393,C222394</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instore</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="13"/>
+        <color rgb="FF797979"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">C222396</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="12"/>
+        <color rgb="FF797979"/>
+        <rFont val=""/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">,</t>
+    </r>
+    <r>
+      <rPr>
+        <i val="true"/>
+        <sz val="13"/>
+        <color rgb="FF797979"/>
+        <rFont val="JetBrains Mono"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">C222937,C222938</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Instore</t>
   </si>
 </sst>
 </file>
@@ -1232,7 +1340,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1290,6 +1398,27 @@
       <color rgb="FF0A4F67"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="13"/>
+      <color rgb="FF797979"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="12"/>
+      <color rgb="FF797979"/>
+      <name val=""/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1369,7 +1498,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1410,6 +1539,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1437,7 +1574,7 @@
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF797979"/>
       <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
@@ -6129,15 +6266,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.4921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.69"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="30.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.95"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6147,13 +6286,97 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>12</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>404</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>405</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>407</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>408</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>410</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>411</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>413</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>414</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>415</v>
       </c>
     </row>
   </sheetData>

</xml_diff>